<commit_message>
Previsoes e numeros atualizados 30/03/2019
</commit_message>
<xml_diff>
--- a/LCK_COREIA_2019.xlsx
+++ b/LCK_COREIA_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA038C64-34C2-4688-9356-04CB4EAAEFDA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B1BF42-5585-4E9E-9670-6BB49F65FCD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Games" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="95">
   <si>
     <t xml:space="preserve">       Semana 1</t>
   </si>
@@ -1382,7 +1382,7 @@
   <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201"/>
+      <selection activeCell="E198" sqref="E198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3588,24 +3588,59 @@
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201" s="74"/>
-      <c r="B201" s="74"/>
+      <c r="A201" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="B201" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="C201" s="81">
+        <v>10</v>
+      </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202" s="74"/>
-      <c r="B202" s="74"/>
+      <c r="A202" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="B202" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="C202" s="81">
+        <v>10</v>
+      </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A203" s="74"/>
-      <c r="B203" s="74"/>
+      <c r="A203" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B203" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="C203" s="81">
+        <v>10</v>
+      </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A204" s="74"/>
-      <c r="B204" s="74"/>
+      <c r="A204" s="74" t="s">
+        <v>84</v>
+      </c>
+      <c r="B204" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C204" s="81">
+        <v>10</v>
+      </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A205" s="74"/>
-      <c r="B205" s="74"/>
+      <c r="A205" s="74" t="s">
+        <v>84</v>
+      </c>
+      <c r="B205" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C205" s="81">
+        <v>10</v>
+      </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="74"/>

</xml_diff>

<commit_message>
Previsoes e numeros atualizados 31/03/2019
</commit_message>
<xml_diff>
--- a/LCK_COREIA_2019.xlsx
+++ b/LCK_COREIA_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B1BF42-5585-4E9E-9670-6BB49F65FCD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A39AF35-063A-468B-A9ED-9AE53FDCD4D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Games" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="95">
   <si>
     <t xml:space="preserve">       Semana 1</t>
   </si>
@@ -887,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1091,6 +1091,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1381,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="E198" sqref="E198"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="F192" sqref="F192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3500,21 +3503,21 @@
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" s="74" t="s">
+      <c r="A193" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="B193" s="74" t="s">
+      <c r="B193" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="C193" s="81">
+      <c r="C193" s="79">
         <v>10</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" s="74" t="s">
+      <c r="A194" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="B194" s="74" t="s">
+      <c r="B194" s="95" t="s">
         <v>85</v>
       </c>
       <c r="C194" s="81">
@@ -3522,10 +3525,10 @@
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" s="74" t="s">
+      <c r="A195" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="B195" s="74" t="s">
+      <c r="B195" s="95" t="s">
         <v>87</v>
       </c>
       <c r="C195" s="81">
@@ -3533,10 +3536,10 @@
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" s="74" t="s">
+      <c r="A196" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="B196" s="74" t="s">
+      <c r="B196" s="95" t="s">
         <v>87</v>
       </c>
       <c r="C196" s="81">
@@ -3544,10 +3547,10 @@
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" s="74" t="s">
+      <c r="A197" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B197" s="74" t="s">
+      <c r="B197" s="95" t="s">
         <v>89</v>
       </c>
       <c r="C197" s="81">
@@ -3555,10 +3558,10 @@
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A198" s="74" t="s">
+      <c r="A198" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B198" s="74" t="s">
+      <c r="B198" s="95" t="s">
         <v>89</v>
       </c>
       <c r="C198" s="81">
@@ -3566,10 +3569,10 @@
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A199" s="74" t="s">
+      <c r="A199" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="B199" s="74" t="s">
+      <c r="B199" s="95" t="s">
         <v>90</v>
       </c>
       <c r="C199" s="81">
@@ -3577,10 +3580,10 @@
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" s="74" t="s">
+      <c r="A200" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="B200" s="74" t="s">
+      <c r="B200" s="95" t="s">
         <v>90</v>
       </c>
       <c r="C200" s="81">
@@ -3588,10 +3591,10 @@
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201" s="74" t="s">
+      <c r="A201" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="B201" s="74" t="s">
+      <c r="B201" s="95" t="s">
         <v>87</v>
       </c>
       <c r="C201" s="81">
@@ -3599,10 +3602,10 @@
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202" s="74" t="s">
+      <c r="A202" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="B202" s="74" t="s">
+      <c r="B202" s="95" t="s">
         <v>87</v>
       </c>
       <c r="C202" s="81">
@@ -3610,10 +3613,10 @@
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A203" s="74" t="s">
+      <c r="A203" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="B203" s="74" t="s">
+      <c r="B203" s="95" t="s">
         <v>92</v>
       </c>
       <c r="C203" s="81">
@@ -3621,10 +3624,10 @@
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A204" s="74" t="s">
+      <c r="A204" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="B204" s="74" t="s">
+      <c r="B204" s="95" t="s">
         <v>93</v>
       </c>
       <c r="C204" s="81">
@@ -3632,10 +3635,10 @@
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A205" s="74" t="s">
+      <c r="A205" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="B205" s="74" t="s">
+      <c r="B205" s="95" t="s">
         <v>93</v>
       </c>
       <c r="C205" s="81">
@@ -3643,78 +3646,106 @@
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A206" s="74"/>
-      <c r="B206" s="74"/>
+      <c r="A206" s="84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B206" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="C206" s="81">
+        <v>10</v>
+      </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A207" s="74"/>
-      <c r="B207" s="74"/>
+      <c r="A207" s="84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B207" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="C207" s="81">
+        <v>10</v>
+      </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A208" s="74"/>
-      <c r="B208" s="74"/>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A209" s="74"/>
-      <c r="B209" s="74"/>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="B208" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="C208" s="81">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A209" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="B209" s="76" t="s">
+        <v>89</v>
+      </c>
+      <c r="C209" s="83">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="74"/>
       <c r="B210" s="74"/>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="74"/>
       <c r="B211" s="74"/>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="74"/>
       <c r="B212" s="74"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="74"/>
       <c r="B213" s="74"/>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="74"/>
       <c r="B214" s="74"/>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="74"/>
       <c r="B215" s="74"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="74"/>
       <c r="B216" s="74"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="74"/>
       <c r="B217" s="74"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="74"/>
       <c r="B218" s="74"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="74"/>
       <c r="B219" s="74"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="74"/>
       <c r="B220" s="74"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="74"/>
       <c r="B221" s="74"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="74"/>
       <c r="B222" s="74"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="74"/>
       <c r="B223" s="74"/>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="74"/>
       <c r="B224" s="74"/>
     </row>

</xml_diff>

<commit_message>
Previsoes, base de dados e numeros atualizados 03/04/2019
</commit_message>
<xml_diff>
--- a/LCK_COREIA_2019.xlsx
+++ b/LCK_COREIA_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A39AF35-063A-468B-A9ED-9AE53FDCD4D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CCEE9F-57C2-4968-B180-B66AB3398068}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="95">
   <si>
     <t xml:space="preserve">       Semana 1</t>
   </si>
@@ -1093,9 +1093,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="F192" sqref="F192"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="C212" sqref="C212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3517,7 +3515,7 @@
       <c r="A194" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="B194" s="95" t="s">
+      <c r="B194" s="74" t="s">
         <v>85</v>
       </c>
       <c r="C194" s="81">
@@ -3528,7 +3526,7 @@
       <c r="A195" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="B195" s="95" t="s">
+      <c r="B195" s="74" t="s">
         <v>87</v>
       </c>
       <c r="C195" s="81">
@@ -3539,7 +3537,7 @@
       <c r="A196" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="B196" s="95" t="s">
+      <c r="B196" s="74" t="s">
         <v>87</v>
       </c>
       <c r="C196" s="81">
@@ -3550,7 +3548,7 @@
       <c r="A197" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B197" s="95" t="s">
+      <c r="B197" s="74" t="s">
         <v>89</v>
       </c>
       <c r="C197" s="81">
@@ -3561,7 +3559,7 @@
       <c r="A198" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B198" s="95" t="s">
+      <c r="B198" s="74" t="s">
         <v>89</v>
       </c>
       <c r="C198" s="81">
@@ -3572,7 +3570,7 @@
       <c r="A199" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="B199" s="95" t="s">
+      <c r="B199" s="74" t="s">
         <v>90</v>
       </c>
       <c r="C199" s="81">
@@ -3583,7 +3581,7 @@
       <c r="A200" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="B200" s="95" t="s">
+      <c r="B200" s="74" t="s">
         <v>90</v>
       </c>
       <c r="C200" s="81">
@@ -3594,7 +3592,7 @@
       <c r="A201" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="B201" s="95" t="s">
+      <c r="B201" s="74" t="s">
         <v>87</v>
       </c>
       <c r="C201" s="81">
@@ -3605,7 +3603,7 @@
       <c r="A202" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="B202" s="95" t="s">
+      <c r="B202" s="74" t="s">
         <v>87</v>
       </c>
       <c r="C202" s="81">
@@ -3616,7 +3614,7 @@
       <c r="A203" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="B203" s="95" t="s">
+      <c r="B203" s="74" t="s">
         <v>92</v>
       </c>
       <c r="C203" s="81">
@@ -3627,7 +3625,7 @@
       <c r="A204" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="B204" s="95" t="s">
+      <c r="B204" s="74" t="s">
         <v>93</v>
       </c>
       <c r="C204" s="81">
@@ -3638,7 +3636,7 @@
       <c r="A205" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="B205" s="95" t="s">
+      <c r="B205" s="74" t="s">
         <v>93</v>
       </c>
       <c r="C205" s="81">
@@ -3649,7 +3647,7 @@
       <c r="A206" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="B206" s="95" t="s">
+      <c r="B206" s="74" t="s">
         <v>85</v>
       </c>
       <c r="C206" s="81">
@@ -3660,7 +3658,7 @@
       <c r="A207" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="B207" s="95" t="s">
+      <c r="B207" s="74" t="s">
         <v>85</v>
       </c>
       <c r="C207" s="81">
@@ -3671,7 +3669,7 @@
       <c r="A208" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="B208" s="95" t="s">
+      <c r="B208" s="74" t="s">
         <v>89</v>
       </c>
       <c r="C208" s="81">
@@ -3690,16 +3688,37 @@
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A210" s="74"/>
-      <c r="B210" s="74"/>
+      <c r="A210" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="B210" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="C210" s="95">
+        <v>-1</v>
+      </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A211" s="74"/>
-      <c r="B211" s="74"/>
+      <c r="A211" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="B211" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="C211" s="95">
+        <v>-1</v>
+      </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A212" s="74"/>
-      <c r="B212" s="74"/>
+      <c r="A212" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="B212" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C212" s="95">
+        <v>-1</v>
+      </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="74"/>

</xml_diff>

<commit_message>
Numeros e dados atualizados 05/04/2019
</commit_message>
<xml_diff>
--- a/LCK_COREIA_2019.xlsx
+++ b/LCK_COREIA_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CCEE9F-57C2-4968-B180-B66AB3398068}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B7684D-25B0-4B74-9D4A-53BB17BC63F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Games" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="95">
   <si>
     <t xml:space="preserve">       Semana 1</t>
   </si>
@@ -887,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1093,7 +1093,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1383,7 +1382,7 @@
   <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="C212" sqref="C212"/>
+      <selection activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3694,7 +3693,7 @@
       <c r="B210" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="C210" s="95">
+      <c r="C210" s="81">
         <v>-1</v>
       </c>
     </row>
@@ -3705,7 +3704,7 @@
       <c r="B211" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="C211" s="95">
+      <c r="C211" s="81">
         <v>-1</v>
       </c>
     </row>
@@ -3716,21 +3715,42 @@
       <c r="B212" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="C212" s="95">
+      <c r="C212" s="81">
         <v>-1</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A213" s="74"/>
-      <c r="B213" s="74"/>
+      <c r="A213" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B213" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C213" s="81">
+        <v>-1</v>
+      </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A214" s="74"/>
-      <c r="B214" s="74"/>
+      <c r="A214" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B214" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C214" s="81">
+        <v>-1</v>
+      </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A215" s="74"/>
-      <c r="B215" s="74"/>
+      <c r="A215" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B215" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C215" s="81">
+        <v>-1</v>
+      </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="74"/>

</xml_diff>